<commit_message>
Repeated a varation using GROUPBY
</commit_message>
<xml_diff>
--- a/CH-123 Custom Grouping.xlsx
+++ b/CH-123 Custom Grouping.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCA59E3-0FC1-485C-9A0A-D9A9B3C4DEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD28F757-50E7-493E-8278-91F9F2465538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
     <sheet name="Alt2" sheetId="4" r:id="rId3"/>
-    <sheet name="Original (2)" sheetId="5" r:id="rId4"/>
+    <sheet name="EDA" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$B$2:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">EDA!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$26</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Original (2)'!$B$2:$D$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="8">
   <si>
     <t>Question</t>
   </si>
@@ -89,11 +89,17 @@
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7248074411692474368/</t>
   </si>
+  <si>
+    <t>Alternative 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;\-0;0;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -365,6 +371,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1317,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{024321D9-7150-4DCC-8957-9558072A52D9}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1711,16 +1718,6 @@
       <c r="C29" t="str">
         <v>Total Sales</v>
       </c>
-      <c r="G29" s="6" t="str" cm="1">
-        <f t="array" ref="G29:H32">_xlfn.LET(
-_xlpm.d,_xlfn.BYROW(_xlfn.WRAPROWS(C3:C26,10,0),_xleta.SUM),
-_xlfn.VSTACK({"Group","Total Sales"},_xlfn.HSTACK({1;2;3},_xlpm.d))
-)</f>
-        <v>Group</v>
-      </c>
-      <c r="H29" s="15" t="str">
-        <v>Total Sales</v>
-      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B30" s="4">
@@ -1729,12 +1726,6 @@
       <c r="C30">
         <v>761</v>
       </c>
-      <c r="G30" s="23">
-        <v>1</v>
-      </c>
-      <c r="H30" s="16">
-        <v>761</v>
-      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
@@ -1743,24 +1734,12 @@
       <c r="C31">
         <v>730</v>
       </c>
-      <c r="G31" s="23">
-        <v>2</v>
-      </c>
-      <c r="H31" s="16">
-        <v>730</v>
-      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B32" s="4">
         <v>3</v>
       </c>
       <c r="C32">
-        <v>385</v>
-      </c>
-      <c r="G32" s="23">
-        <v>3</v>
-      </c>
-      <c r="H32" s="16">
         <v>385</v>
       </c>
     </row>
@@ -2197,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A358D79B-6569-4ACB-A563-1D8BF6250203}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2210,6 +2189,7 @@
     <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="4.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2574,6 +2554,71 @@
         <v>105</v>
       </c>
       <c r="D26" s="9"/>
+      <c r="G26" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="28"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G28" s="6" t="str" cm="1">
+        <f t="array" ref="G28:H31">_xlfn.LET(
+_xlpm.d,_xlfn.BYROW(_xlfn.WRAPROWS('Alt1'!C3:C26,10,0),_xleta.SUM),
+_xlfn.VSTACK({"Group","Total Sales"},_xlfn.HSTACK({1;2;3},_xlpm.d))
+)</f>
+        <v>Group</v>
+      </c>
+      <c r="H28" s="15" t="str">
+        <v>Total Sales</v>
+      </c>
+      <c r="J28" s="6" t="str" cm="1">
+        <f t="array" ref="J28:K31">_xlfn.VSTACK({"Group","Total Sales"},_xlfn.GROUPBY(QUOTIENT(B3:B26-$B$3,10),C3:C26,_xleta.SUM,,0))</f>
+        <v>Group</v>
+      </c>
+      <c r="K28" s="15" t="str">
+        <v>Total Sales</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G29" s="23">
+        <v>1</v>
+      </c>
+      <c r="H29" s="16">
+        <v>761</v>
+      </c>
+      <c r="J29" s="23">
+        <v>0</v>
+      </c>
+      <c r="K29" s="16">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G30" s="23">
+        <v>2</v>
+      </c>
+      <c r="H30" s="16">
+        <v>730</v>
+      </c>
+      <c r="J30" s="23">
+        <v>1</v>
+      </c>
+      <c r="K30" s="16">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G31" s="23">
+        <v>3</v>
+      </c>
+      <c r="H31" s="16">
+        <v>385</v>
+      </c>
+      <c r="J31" s="23">
+        <v>2</v>
+      </c>
+      <c r="K31" s="16">
+        <v>385</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>